<commit_message>
update predict by excel and funtion train model
</commit_message>
<xml_diff>
--- a/data/LR_Actual_Pred_TN.xlsx
+++ b/data/LR_Actual_Pred_TN.xlsx
@@ -500,37 +500,37 @@
         <v>7.8</v>
       </c>
       <c r="B2" t="n">
-        <v>7.203265315540123</v>
+        <v>7.734822300544285</v>
       </c>
       <c r="C2" t="n">
         <v>7.5</v>
       </c>
       <c r="D2" t="n">
-        <v>7.536188996190657</v>
+        <v>7.154045140381974</v>
       </c>
       <c r="E2" t="n">
         <v>4.25</v>
       </c>
       <c r="F2" t="n">
-        <v>6.478266445569433</v>
+        <v>6.159382983073893</v>
       </c>
       <c r="G2" t="n">
         <v>6.5</v>
       </c>
       <c r="H2" t="n">
-        <v>6.896006168185369</v>
+        <v>7.498400070281096</v>
       </c>
       <c r="I2" t="n">
         <v>4</v>
       </c>
       <c r="J2" t="n">
-        <v>5.528753724568377</v>
+        <v>5.624590986925111</v>
       </c>
       <c r="K2" t="n">
         <v>4.6</v>
       </c>
       <c r="L2" t="n">
-        <v>6.210178508581591</v>
+        <v>6.064799162992669</v>
       </c>
     </row>
     <row r="3">
@@ -538,37 +538,37 @@
         <v>8.199999999999999</v>
       </c>
       <c r="B3" t="n">
-        <v>7.287551100005455</v>
+        <v>7.786191744810006</v>
       </c>
       <c r="C3" t="n">
         <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>7.3062480762374</v>
+        <v>6.855449627933415</v>
       </c>
       <c r="E3" t="n">
         <v>7.75</v>
       </c>
       <c r="F3" t="n">
-        <v>6.927600125596583</v>
+        <v>6.701528374275473</v>
       </c>
       <c r="G3" t="n">
         <v>8.75</v>
       </c>
       <c r="H3" t="n">
-        <v>7.478765397644307</v>
+        <v>8.075204493679998</v>
       </c>
       <c r="I3" t="n">
         <v>5.75</v>
       </c>
       <c r="J3" t="n">
-        <v>5.308233156799145</v>
+        <v>5.319142389300846</v>
       </c>
       <c r="K3" t="n">
         <v>7.6</v>
       </c>
       <c r="L3" t="n">
-        <v>6.823701548167713</v>
+        <v>6.69211052828005</v>
       </c>
     </row>
     <row r="4">
@@ -576,37 +576,37 @@
         <v>8.6</v>
       </c>
       <c r="B4" t="n">
-        <v>7.70287079317127</v>
+        <v>8.238363511072729</v>
       </c>
       <c r="C4" t="n">
         <v>8.75</v>
       </c>
       <c r="D4" t="n">
-        <v>7.846375104031123</v>
+        <v>7.448701168985183</v>
       </c>
       <c r="E4" t="n">
         <v>5.5</v>
       </c>
       <c r="F4" t="n">
-        <v>6.792084461848653</v>
+        <v>6.555677986570237</v>
       </c>
       <c r="G4" t="n">
         <v>8.75</v>
       </c>
       <c r="H4" t="n">
-        <v>7.097033387851208</v>
+        <v>7.709916827562402</v>
       </c>
       <c r="I4" t="n">
         <v>7</v>
       </c>
       <c r="J4" t="n">
-        <v>6.788327149929615</v>
+        <v>6.805821688796094</v>
       </c>
       <c r="K4" t="n">
         <v>6.2</v>
       </c>
       <c r="L4" t="n">
-        <v>6.640624072469355</v>
+        <v>6.487157631730529</v>
       </c>
     </row>
     <row r="5">
@@ -614,37 +614,37 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>6.776529175334253</v>
+        <v>7.274974767332071</v>
       </c>
       <c r="C5" t="n">
         <v>7</v>
       </c>
       <c r="D5" t="n">
-        <v>7.05916875680485</v>
+        <v>6.665379369038885</v>
       </c>
       <c r="E5" t="n">
         <v>5.5</v>
       </c>
       <c r="F5" t="n">
-        <v>5.954025407825379</v>
+        <v>5.449682285130847</v>
       </c>
       <c r="G5" t="n">
         <v>6.25</v>
       </c>
       <c r="H5" t="n">
-        <v>6.301036795948366</v>
+        <v>6.831628971627622</v>
       </c>
       <c r="I5" t="n">
         <v>5.25</v>
       </c>
       <c r="J5" t="n">
-        <v>5.107923120539597</v>
+        <v>5.22951335436858</v>
       </c>
       <c r="K5" t="n">
         <v>5</v>
       </c>
       <c r="L5" t="n">
-        <v>6.295342488667475</v>
+        <v>6.065460675451611</v>
       </c>
     </row>
     <row r="6">
@@ -652,37 +652,37 @@
         <v>6.8</v>
       </c>
       <c r="B6" t="n">
-        <v>6.925932466207101</v>
+        <v>7.459674920937993</v>
       </c>
       <c r="C6" t="n">
         <v>6.5</v>
       </c>
       <c r="D6" t="n">
-        <v>7.543836430347094</v>
+        <v>7.17528299831811</v>
       </c>
       <c r="E6" t="n">
         <v>5.75</v>
       </c>
       <c r="F6" t="n">
-        <v>6.425639288423715</v>
+        <v>6.125506744387467</v>
       </c>
       <c r="G6" t="n">
         <v>6.25</v>
       </c>
       <c r="H6" t="n">
-        <v>6.339401350219654</v>
+        <v>6.905536091905366</v>
       </c>
       <c r="I6" t="n">
         <v>6</v>
       </c>
       <c r="J6" t="n">
-        <v>4.990307728513375</v>
+        <v>4.924165538003804</v>
       </c>
       <c r="K6" t="n">
         <v>4.4</v>
       </c>
       <c r="L6" t="n">
-        <v>5.649498166256029</v>
+        <v>5.491777725752428</v>
       </c>
     </row>
     <row r="7">
@@ -690,37 +690,37 @@
         <v>8.199999999999999</v>
       </c>
       <c r="B7" t="n">
-        <v>6.713287818060299</v>
+        <v>7.241730877625742</v>
       </c>
       <c r="C7" t="n">
         <v>8</v>
       </c>
       <c r="D7" t="n">
-        <v>7.582880585419597</v>
+        <v>7.204850688403015</v>
       </c>
       <c r="E7" t="n">
         <v>7.25</v>
       </c>
       <c r="F7" t="n">
-        <v>6.354393157870383</v>
+        <v>6.046835325504549</v>
       </c>
       <c r="G7" t="n">
         <v>7.75</v>
       </c>
       <c r="H7" t="n">
-        <v>4.761734149095169</v>
+        <v>5.329047740918485</v>
       </c>
       <c r="I7" t="n">
         <v>7.5</v>
       </c>
       <c r="J7" t="n">
-        <v>3.978276935091878</v>
+        <v>4.112214091262083</v>
       </c>
       <c r="K7" t="n">
         <v>6</v>
       </c>
       <c r="L7" t="n">
-        <v>4.482148917354014</v>
+        <v>4.338624207848459</v>
       </c>
     </row>
     <row r="8">
@@ -728,37 +728,37 @@
         <v>7.4</v>
       </c>
       <c r="B8" t="n">
-        <v>6.951343453071942</v>
+        <v>7.507408018585941</v>
       </c>
       <c r="C8" t="n">
         <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>7.699784514167287</v>
+        <v>7.377920532450686</v>
       </c>
       <c r="E8" t="n">
         <v>6.5</v>
       </c>
       <c r="F8" t="n">
-        <v>7.505121400437393</v>
+        <v>7.702416138431997</v>
       </c>
       <c r="G8" t="n">
         <v>7</v>
       </c>
       <c r="H8" t="n">
-        <v>7.541578034017293</v>
+        <v>8.156264400968666</v>
       </c>
       <c r="I8" t="n">
         <v>4</v>
       </c>
       <c r="J8" t="n">
-        <v>5.067028408091477</v>
+        <v>5.02229316604477</v>
       </c>
       <c r="K8" t="n">
         <v>7.8</v>
       </c>
       <c r="L8" t="n">
-        <v>6.253687854921912</v>
+        <v>6.211186258486341</v>
       </c>
     </row>
     <row r="9">
@@ -766,37 +766,37 @@
         <v>6.4</v>
       </c>
       <c r="B9" t="n">
-        <v>5.908424058660479</v>
+        <v>6.441770495559333</v>
       </c>
       <c r="C9" t="n">
         <v>6.25</v>
       </c>
       <c r="D9" t="n">
-        <v>7.137343544716613</v>
+        <v>6.737322893839197</v>
       </c>
       <c r="E9" t="n">
         <v>4.75</v>
       </c>
       <c r="F9" t="n">
-        <v>5.807349452773504</v>
+        <v>5.476921802679703</v>
       </c>
       <c r="G9" t="n">
         <v>6</v>
       </c>
       <c r="H9" t="n">
-        <v>5.375322902168641</v>
+        <v>5.945413748862594</v>
       </c>
       <c r="I9" t="n">
         <v>4</v>
       </c>
       <c r="J9" t="n">
-        <v>3.840219138362716</v>
+        <v>4.032543725019099</v>
       </c>
       <c r="K9" t="n">
         <v>6</v>
       </c>
       <c r="L9" t="n">
-        <v>5.018153637615403</v>
+        <v>4.979347790788426</v>
       </c>
     </row>
     <row r="10">
@@ -804,37 +804,37 @@
         <v>7.6</v>
       </c>
       <c r="B10" t="n">
-        <v>7.745909970405318</v>
+        <v>8.20273459475959</v>
       </c>
       <c r="C10" t="n">
         <v>7.5</v>
       </c>
       <c r="D10" t="n">
-        <v>7.744623646533536</v>
+        <v>7.305180761431156</v>
       </c>
       <c r="E10" t="n">
         <v>5.75</v>
       </c>
       <c r="F10" t="n">
-        <v>6.434516617571224</v>
+        <v>5.971450679567277</v>
       </c>
       <c r="G10" t="n">
         <v>8.75</v>
       </c>
       <c r="H10" t="n">
-        <v>7.35335053360703</v>
+        <v>7.881596240817777</v>
       </c>
       <c r="I10" t="n">
         <v>9.25</v>
       </c>
       <c r="J10" t="n">
-        <v>6.825755386813228</v>
+        <v>6.726778518909979</v>
       </c>
       <c r="K10" t="n">
         <v>6.4</v>
       </c>
       <c r="L10" t="n">
-        <v>7.134468857877733</v>
+        <v>6.882518926348467</v>
       </c>
     </row>
     <row r="11">
@@ -842,37 +842,37 @@
         <v>8</v>
       </c>
       <c r="B11" t="n">
-        <v>6.687742640547324</v>
+        <v>7.20680603933756</v>
       </c>
       <c r="C11" t="n">
         <v>6.75</v>
       </c>
       <c r="D11" t="n">
-        <v>7.088577502555108</v>
+        <v>6.585428576880131</v>
       </c>
       <c r="E11" t="n">
         <v>7.75</v>
       </c>
       <c r="F11" t="n">
-        <v>6.925703311437597</v>
+        <v>6.928943470383333</v>
       </c>
       <c r="G11" t="n">
         <v>7.25</v>
       </c>
       <c r="H11" t="n">
-        <v>6.601401320638017</v>
+        <v>7.266358833428964</v>
       </c>
       <c r="I11" t="n">
         <v>6.5</v>
       </c>
       <c r="J11" t="n">
-        <v>4.601455139326202</v>
+        <v>4.658767807279414</v>
       </c>
       <c r="K11" t="n">
         <v>7.8</v>
       </c>
       <c r="L11" t="n">
-        <v>8.559244661888096</v>
+        <v>8.402963561143014</v>
       </c>
     </row>
     <row r="12">
@@ -880,37 +880,37 @@
         <v>7.8</v>
       </c>
       <c r="B12" t="n">
-        <v>7.194009352270761</v>
+        <v>7.69917891365011</v>
       </c>
       <c r="C12" t="n">
         <v>8.5</v>
       </c>
       <c r="D12" t="n">
-        <v>8.345344604844666</v>
+        <v>8.015762139515722</v>
       </c>
       <c r="E12" t="n">
         <v>7.5</v>
       </c>
       <c r="F12" t="n">
-        <v>6.540385845595593</v>
+        <v>6.306637132115532</v>
       </c>
       <c r="G12" t="n">
         <v>8.5</v>
       </c>
       <c r="H12" t="n">
-        <v>6.789188464081604</v>
+        <v>7.443327003655896</v>
       </c>
       <c r="I12" t="n">
         <v>6.25</v>
       </c>
       <c r="J12" t="n">
-        <v>6.509190425506286</v>
+        <v>6.437824929048448</v>
       </c>
       <c r="K12" t="n">
         <v>6</v>
       </c>
       <c r="L12" t="n">
-        <v>6.222014898888614</v>
+        <v>6.062591631784088</v>
       </c>
     </row>
     <row r="13">
@@ -918,37 +918,37 @@
         <v>8.6</v>
       </c>
       <c r="B13" t="n">
-        <v>7.86695416281473</v>
+        <v>8.363073235822439</v>
       </c>
       <c r="C13" t="n">
         <v>8.5</v>
       </c>
       <c r="D13" t="n">
-        <v>8.582016416313149</v>
+        <v>8.275730315553336</v>
       </c>
       <c r="E13" t="n">
         <v>8.75</v>
       </c>
       <c r="F13" t="n">
-        <v>7.305402539968623</v>
+        <v>7.335273047607182</v>
       </c>
       <c r="G13" t="n">
         <v>7</v>
       </c>
       <c r="H13" t="n">
-        <v>6.951513898628763</v>
+        <v>7.612645395938199</v>
       </c>
       <c r="I13" t="n">
         <v>6.25</v>
       </c>
       <c r="J13" t="n">
-        <v>5.72094073325374</v>
+        <v>5.645647067338111</v>
       </c>
       <c r="K13" t="n">
         <v>6</v>
       </c>
       <c r="L13" t="n">
-        <v>6.36225295723666</v>
+        <v>6.23197463623109</v>
       </c>
     </row>
     <row r="14">
@@ -956,37 +956,37 @@
         <v>7.8</v>
       </c>
       <c r="B14" t="n">
-        <v>7.709949219422128</v>
+        <v>8.240589444815917</v>
       </c>
       <c r="C14" t="n">
         <v>8.25</v>
       </c>
       <c r="D14" t="n">
-        <v>8.069834976288783</v>
+        <v>7.719497567531945</v>
       </c>
       <c r="E14" t="n">
         <v>6</v>
       </c>
       <c r="F14" t="n">
-        <v>6.616761001510711</v>
+        <v>6.372391630978683</v>
       </c>
       <c r="G14" t="n">
         <v>8.5</v>
       </c>
       <c r="H14" t="n">
-        <v>6.734337796882099</v>
+        <v>7.355456712767419</v>
       </c>
       <c r="I14" t="n">
         <v>5.75</v>
       </c>
       <c r="J14" t="n">
-        <v>5.985068048992627</v>
+        <v>5.97278238176141</v>
       </c>
       <c r="K14" t="n">
         <v>8.199999999999999</v>
       </c>
       <c r="L14" t="n">
-        <v>6.889155523560714</v>
+        <v>6.715670717082867</v>
       </c>
     </row>
     <row r="15">
@@ -994,37 +994,37 @@
         <v>8</v>
       </c>
       <c r="B15" t="n">
-        <v>7.649692825890418</v>
+        <v>8.129667607377094</v>
       </c>
       <c r="C15" t="n">
         <v>8.75</v>
       </c>
       <c r="D15" t="n">
-        <v>8.409494688259862</v>
+        <v>8.097449604464051</v>
       </c>
       <c r="E15" t="n">
         <v>7.5</v>
       </c>
       <c r="F15" t="n">
-        <v>7.026138493310958</v>
+        <v>6.883716777789544</v>
       </c>
       <c r="G15" t="n">
         <v>6.75</v>
       </c>
       <c r="H15" t="n">
-        <v>6.817353124558143</v>
+        <v>7.435333651797741</v>
       </c>
       <c r="I15" t="n">
         <v>5.25</v>
       </c>
       <c r="J15" t="n">
-        <v>5.469731319843097</v>
+        <v>5.475464090970185</v>
       </c>
       <c r="K15" t="n">
         <v>6.2</v>
       </c>
       <c r="L15" t="n">
-        <v>6.347001991855618</v>
+        <v>6.249800349422525</v>
       </c>
     </row>
     <row r="16">
@@ -1032,37 +1032,37 @@
         <v>7.6</v>
       </c>
       <c r="B16" t="n">
-        <v>6.529017129650729</v>
+        <v>7.043057316705903</v>
       </c>
       <c r="C16" t="n">
         <v>9</v>
       </c>
       <c r="D16" t="n">
-        <v>7.987298275418884</v>
+        <v>7.611684341103365</v>
       </c>
       <c r="E16" t="n">
         <v>7</v>
       </c>
       <c r="F16" t="n">
-        <v>5.913484636681017</v>
+        <v>5.467176351709571</v>
       </c>
       <c r="G16" t="n">
         <v>7.25</v>
       </c>
       <c r="H16" t="n">
-        <v>7.292661196151398</v>
+        <v>7.939216028208435</v>
       </c>
       <c r="I16" t="n">
         <v>4.25</v>
       </c>
       <c r="J16" t="n">
-        <v>4.475413601249882</v>
+        <v>4.474432427794937</v>
       </c>
       <c r="K16" t="n">
         <v>9</v>
       </c>
       <c r="L16" t="n">
-        <v>7.951822862990745</v>
+        <v>7.741439014091265</v>
       </c>
     </row>
     <row r="17">
@@ -1070,37 +1070,37 @@
         <v>7.4</v>
       </c>
       <c r="B17" t="n">
-        <v>6.450921206922933</v>
+        <v>6.976684108211383</v>
       </c>
       <c r="C17" t="n">
         <v>8.5</v>
       </c>
       <c r="D17" t="n">
-        <v>7.87142428940056</v>
+        <v>7.491201795866358</v>
       </c>
       <c r="E17" t="n">
         <v>6.25</v>
       </c>
       <c r="F17" t="n">
-        <v>5.915855934322862</v>
+        <v>5.460702492013891</v>
       </c>
       <c r="G17" t="n">
         <v>7.25</v>
       </c>
       <c r="H17" t="n">
-        <v>6.563069499704877</v>
+        <v>7.138827548778433</v>
       </c>
       <c r="I17" t="n">
         <v>6.5</v>
       </c>
       <c r="J17" t="n">
-        <v>3.935439475163843</v>
+        <v>3.888461616927755</v>
       </c>
       <c r="K17" t="n">
         <v>6.8</v>
       </c>
       <c r="L17" t="n">
-        <v>5.665021819388245</v>
+        <v>5.627812899660171</v>
       </c>
     </row>
     <row r="18">
@@ -1108,37 +1108,37 @@
         <v>7.8</v>
       </c>
       <c r="B18" t="n">
-        <v>7.157864000615823</v>
+        <v>7.672668397353151</v>
       </c>
       <c r="C18" t="n">
         <v>8</v>
       </c>
       <c r="D18" t="n">
-        <v>7.654391981864553</v>
+        <v>7.229397391942529</v>
       </c>
       <c r="E18" t="n">
         <v>6.5</v>
       </c>
       <c r="F18" t="n">
-        <v>6.174003826200818</v>
+        <v>5.860658031132187</v>
       </c>
       <c r="G18" t="n">
         <v>8.25</v>
       </c>
       <c r="H18" t="n">
-        <v>6.424816842417669</v>
+        <v>7.038989601444717</v>
       </c>
       <c r="I18" t="n">
         <v>8</v>
       </c>
       <c r="J18" t="n">
-        <v>6.818823251201729</v>
+        <v>6.880676434119547</v>
       </c>
       <c r="K18" t="n">
         <v>7</v>
       </c>
       <c r="L18" t="n">
-        <v>7.090558495721344</v>
+        <v>6.941250325762121</v>
       </c>
     </row>
     <row r="19">
@@ -1146,37 +1146,37 @@
         <v>8</v>
       </c>
       <c r="B19" t="n">
-        <v>7.138542770478823</v>
+        <v>7.609545377515938</v>
       </c>
       <c r="C19" t="n">
         <v>8</v>
       </c>
       <c r="D19" t="n">
-        <v>7.62314674365077</v>
+        <v>7.250630295799809</v>
       </c>
       <c r="E19" t="n">
         <v>6.75</v>
       </c>
       <c r="F19" t="n">
-        <v>6.790831406801831</v>
+        <v>6.509122305140752</v>
       </c>
       <c r="G19" t="n">
         <v>5.25</v>
       </c>
       <c r="H19" t="n">
-        <v>6.481521676812263</v>
+        <v>7.013041867663141</v>
       </c>
       <c r="I19" t="n">
         <v>2.75</v>
       </c>
       <c r="J19" t="n">
-        <v>5.288235010749288</v>
+        <v>5.267716304309372</v>
       </c>
       <c r="K19" t="n">
         <v>5.6</v>
       </c>
       <c r="L19" t="n">
-        <v>6.601201082684227</v>
+        <v>6.356385519184597</v>
       </c>
     </row>
     <row r="20">
@@ -1184,37 +1184,37 @@
         <v>7.6</v>
       </c>
       <c r="B20" t="n">
-        <v>7.851744936049385</v>
+        <v>8.322502003413645</v>
       </c>
       <c r="C20" t="n">
         <v>8.75</v>
       </c>
       <c r="D20" t="n">
-        <v>8.257095784787566</v>
+        <v>7.897715160472149</v>
       </c>
       <c r="E20" t="n">
         <v>8.25</v>
       </c>
       <c r="F20" t="n">
-        <v>7.985127231361371</v>
+        <v>8.127208725227106</v>
       </c>
       <c r="G20" t="n">
         <v>8.25</v>
       </c>
       <c r="H20" t="n">
-        <v>7.936476358878484</v>
+        <v>8.543081549556698</v>
       </c>
       <c r="I20" t="n">
         <v>6.75</v>
       </c>
       <c r="J20" t="n">
-        <v>6.677518615731224</v>
+        <v>6.404802228852111</v>
       </c>
       <c r="K20" t="n">
         <v>8.800000000000001</v>
       </c>
       <c r="L20" t="n">
-        <v>8.142068697375398</v>
+        <v>7.711095638550434</v>
       </c>
     </row>
     <row r="21">
@@ -1222,37 +1222,37 @@
         <v>6.8</v>
       </c>
       <c r="B21" t="n">
-        <v>6.964839202407145</v>
+        <v>7.533622449390756</v>
       </c>
       <c r="C21" t="n">
         <v>8.75</v>
       </c>
       <c r="D21" t="n">
-        <v>8.063003442813075</v>
+        <v>7.864828403594625</v>
       </c>
       <c r="E21" t="n">
         <v>6</v>
       </c>
       <c r="F21" t="n">
-        <v>6.167284547364715</v>
+        <v>5.872911107621313</v>
       </c>
       <c r="G21" t="n">
         <v>6</v>
       </c>
       <c r="H21" t="n">
-        <v>6.522494943463772</v>
+        <v>7.117900011465461</v>
       </c>
       <c r="I21" t="n">
         <v>5.25</v>
       </c>
       <c r="J21" t="n">
-        <v>5.433976204972926</v>
+        <v>5.536895747761588</v>
       </c>
       <c r="K21" t="n">
         <v>5</v>
       </c>
       <c r="L21" t="n">
-        <v>4.8916377405337</v>
+        <v>4.905798371423987</v>
       </c>
     </row>
     <row r="22">
@@ -1260,37 +1260,37 @@
         <v>7.8</v>
       </c>
       <c r="B22" t="n">
-        <v>7.076212437354062</v>
+        <v>7.639616590626775</v>
       </c>
       <c r="C22" t="n">
         <v>8.25</v>
       </c>
       <c r="D22" t="n">
-        <v>8.115954962184958</v>
+        <v>7.811783611787443</v>
       </c>
       <c r="E22" t="n">
         <v>4.75</v>
       </c>
       <c r="F22" t="n">
-        <v>6.855744432240988</v>
+        <v>6.745696657088566</v>
       </c>
       <c r="G22" t="n">
         <v>7</v>
       </c>
       <c r="H22" t="n">
-        <v>8.514616021044807</v>
+        <v>9.143123703876253</v>
       </c>
       <c r="I22" t="n">
         <v>5</v>
       </c>
       <c r="J22" t="n">
-        <v>6.149792618379269</v>
+        <v>6.05041721718273</v>
       </c>
       <c r="K22" t="n">
         <v>4</v>
       </c>
       <c r="L22" t="n">
-        <v>6.745533763754838</v>
+        <v>6.532367197229803</v>
       </c>
     </row>
     <row r="23">
@@ -1298,37 +1298,37 @@
         <v>8.6</v>
       </c>
       <c r="B23" t="n">
-        <v>7.914841334552535</v>
+        <v>8.405063869009918</v>
       </c>
       <c r="C23" t="n">
         <v>7.75</v>
       </c>
       <c r="D23" t="n">
-        <v>8.302454119929152</v>
+        <v>8.017611267148332</v>
       </c>
       <c r="E23" t="n">
         <v>7.25</v>
       </c>
       <c r="F23" t="n">
-        <v>7.56236291073861</v>
+        <v>7.527983433923024</v>
       </c>
       <c r="G23" t="n">
         <v>7.75</v>
       </c>
       <c r="H23" t="n">
-        <v>7.317390451866284</v>
+        <v>7.943948947632985</v>
       </c>
       <c r="I23" t="n">
         <v>6.25</v>
       </c>
       <c r="J23" t="n">
-        <v>5.808934036403132</v>
+        <v>5.776611267521668</v>
       </c>
       <c r="K23" t="n">
         <v>4.8</v>
       </c>
       <c r="L23" t="n">
-        <v>6.289935421197614</v>
+        <v>6.202814729828241</v>
       </c>
     </row>
     <row r="24">
@@ -1336,37 +1336,37 @@
         <v>7.8</v>
       </c>
       <c r="B24" t="n">
-        <v>7.230427280512076</v>
+        <v>7.793360089868759</v>
       </c>
       <c r="C24" t="n">
         <v>6.75</v>
       </c>
       <c r="D24" t="n">
-        <v>7.715709486402194</v>
+        <v>7.39594086217322</v>
       </c>
       <c r="E24" t="n">
         <v>7.25</v>
       </c>
       <c r="F24" t="n">
-        <v>6.523878088269446</v>
+        <v>6.363329198673591</v>
       </c>
       <c r="G24" t="n">
         <v>6.75</v>
       </c>
       <c r="H24" t="n">
-        <v>6.457875832997353</v>
+        <v>7.036108266682162</v>
       </c>
       <c r="I24" t="n">
         <v>5.25</v>
       </c>
       <c r="J24" t="n">
-        <v>5.373528534125875</v>
+        <v>5.499453091578809</v>
       </c>
       <c r="K24" t="n">
         <v>4</v>
       </c>
       <c r="L24" t="n">
-        <v>5.065902235315197</v>
+        <v>5.075462746799865</v>
       </c>
     </row>
     <row r="25">
@@ -1374,37 +1374,37 @@
         <v>8.199999999999999</v>
       </c>
       <c r="B25" t="n">
-        <v>6.609453611366897</v>
+        <v>7.232685736929225</v>
       </c>
       <c r="C25" t="n">
         <v>6</v>
       </c>
       <c r="D25" t="n">
-        <v>7.099200269693101</v>
+        <v>6.629252012689296</v>
       </c>
       <c r="E25" t="n">
         <v>6.5</v>
       </c>
       <c r="F25" t="n">
-        <v>6.055002578607571</v>
+        <v>5.801253612098126</v>
       </c>
       <c r="G25" t="n">
         <v>8</v>
       </c>
       <c r="H25" t="n">
-        <v>6.067622294639306</v>
+        <v>6.598848504406877</v>
       </c>
       <c r="I25" t="n">
         <v>6.25</v>
       </c>
       <c r="J25" t="n">
-        <v>5.534946639584455</v>
+        <v>5.673781453420128</v>
       </c>
       <c r="K25" t="n">
         <v>5.6</v>
       </c>
       <c r="L25" t="n">
-        <v>4.921841838461238</v>
+        <v>5.048562818760624</v>
       </c>
     </row>
     <row r="26">
@@ -1412,37 +1412,37 @@
         <v>7.4</v>
       </c>
       <c r="B26" t="n">
-        <v>6.592282618340804</v>
+        <v>7.132439334003144</v>
       </c>
       <c r="C26" t="n">
         <v>7.25</v>
       </c>
       <c r="D26" t="n">
-        <v>7.571639395405914</v>
+        <v>7.194337203733963</v>
       </c>
       <c r="E26" t="n">
         <v>6.75</v>
       </c>
       <c r="F26" t="n">
-        <v>5.597788412633943</v>
+        <v>5.088935318376307</v>
       </c>
       <c r="G26" t="n">
         <v>6.75</v>
       </c>
       <c r="H26" t="n">
-        <v>5.83010818930848</v>
+        <v>6.410575284845548</v>
       </c>
       <c r="I26" t="n">
         <v>4.25</v>
       </c>
       <c r="J26" t="n">
-        <v>4.069877735374448</v>
+        <v>4.207974640973741</v>
       </c>
       <c r="K26" t="n">
         <v>4.6</v>
       </c>
       <c r="L26" t="n">
-        <v>5.070296175648757</v>
+        <v>4.999106256963782</v>
       </c>
     </row>
     <row r="27">
@@ -1450,37 +1450,37 @@
         <v>8.199999999999999</v>
       </c>
       <c r="B27" t="n">
-        <v>6.972708026531249</v>
+        <v>7.49878031351643</v>
       </c>
       <c r="C27" t="n">
         <v>9</v>
       </c>
       <c r="D27" t="n">
-        <v>9.210191525813123</v>
+        <v>9.029659610060897</v>
       </c>
       <c r="E27" t="n">
         <v>7.25</v>
       </c>
       <c r="F27" t="n">
-        <v>6.443636111000974</v>
+        <v>6.231127314065209</v>
       </c>
       <c r="G27" t="n">
         <v>7.5</v>
       </c>
       <c r="H27" t="n">
-        <v>6.971363339354625</v>
+        <v>7.66334598376787</v>
       </c>
       <c r="I27" t="n">
         <v>6.25</v>
       </c>
       <c r="J27" t="n">
-        <v>5.964742755977837</v>
+        <v>5.951726264799442</v>
       </c>
       <c r="K27" t="n">
         <v>5.4</v>
       </c>
       <c r="L27" t="n">
-        <v>4.773636733902919</v>
+        <v>4.751447994375464</v>
       </c>
     </row>
     <row r="28">
@@ -1488,37 +1488,37 @@
         <v>8.6</v>
       </c>
       <c r="B28" t="n">
-        <v>8.061204674755272</v>
+        <v>8.519638248061849</v>
       </c>
       <c r="C28" t="n">
         <v>9</v>
       </c>
       <c r="D28" t="n">
-        <v>8.024300702702398</v>
+        <v>7.544167209378861</v>
       </c>
       <c r="E28" t="n">
         <v>7</v>
       </c>
       <c r="F28" t="n">
-        <v>6.642206651450951</v>
+        <v>6.275621343036888</v>
       </c>
       <c r="G28" t="n">
         <v>8.75</v>
       </c>
       <c r="H28" t="n">
-        <v>7.499296558453277</v>
+        <v>8.073731656065711</v>
       </c>
       <c r="I28" t="n">
         <v>7.25</v>
       </c>
       <c r="J28" t="n">
-        <v>7.898510867385709</v>
+        <v>7.681494746391293</v>
       </c>
       <c r="K28" t="n">
         <v>7.4</v>
       </c>
       <c r="L28" t="n">
-        <v>6.664539788269356</v>
+        <v>6.442923500336022</v>
       </c>
     </row>
     <row r="29">
@@ -1526,37 +1526,37 @@
         <v>6.4</v>
       </c>
       <c r="B29" t="n">
-        <v>6.830477914266813</v>
+        <v>7.387798495933174</v>
       </c>
       <c r="C29" t="n">
         <v>7.5</v>
       </c>
       <c r="D29" t="n">
-        <v>7.395628566469322</v>
+        <v>6.998451402821447</v>
       </c>
       <c r="E29" t="n">
         <v>5.75</v>
       </c>
       <c r="F29" t="n">
-        <v>5.711988099369878</v>
+        <v>5.252071911279724</v>
       </c>
       <c r="G29" t="n">
         <v>7.5</v>
       </c>
       <c r="H29" t="n">
-        <v>6.629254042310732</v>
+        <v>7.258399167539652</v>
       </c>
       <c r="I29" t="n">
         <v>5</v>
       </c>
       <c r="J29" t="n">
-        <v>4.464338483586624</v>
+        <v>4.500350881611412</v>
       </c>
       <c r="K29" t="n">
         <v>5</v>
       </c>
       <c r="L29" t="n">
-        <v>4.166809522115134</v>
+        <v>4.233959082734034</v>
       </c>
     </row>
     <row r="30">
@@ -1564,37 +1564,37 @@
         <v>8.4</v>
       </c>
       <c r="B30" t="n">
-        <v>7.796455663187425</v>
+        <v>8.311250093141675</v>
       </c>
       <c r="C30" t="n">
         <v>7.75</v>
       </c>
       <c r="D30" t="n">
-        <v>8.665506733535587</v>
+        <v>8.30780331851858</v>
       </c>
       <c r="E30" t="n">
         <v>4.75</v>
       </c>
       <c r="F30" t="n">
-        <v>6.641449076672727</v>
+        <v>6.333963472490808</v>
       </c>
       <c r="G30" t="n">
         <v>7.25</v>
       </c>
       <c r="H30" t="n">
-        <v>7.336431487163312</v>
+        <v>7.929789502061464</v>
       </c>
       <c r="I30" t="n">
         <v>8</v>
       </c>
       <c r="J30" t="n">
-        <v>8.475454067776845</v>
+        <v>8.326956513203731</v>
       </c>
       <c r="K30" t="n">
         <v>5</v>
       </c>
       <c r="L30" t="n">
-        <v>5.396099847995369</v>
+        <v>5.326457715218463</v>
       </c>
     </row>
     <row r="31">
@@ -1602,37 +1602,37 @@
         <v>6.2</v>
       </c>
       <c r="B31" t="n">
-        <v>6.787452879536699</v>
+        <v>7.293142576265493</v>
       </c>
       <c r="C31" t="n">
         <v>7</v>
       </c>
       <c r="D31" t="n">
-        <v>7.36455658454727</v>
+        <v>6.948319401132638</v>
       </c>
       <c r="E31" t="n">
         <v>5.5</v>
       </c>
       <c r="F31" t="n">
-        <v>5.538655580178946</v>
+        <v>4.942400501527745</v>
       </c>
       <c r="G31" t="n">
         <v>6.5</v>
       </c>
       <c r="H31" t="n">
-        <v>6.554378100557397</v>
+        <v>7.139342546315605</v>
       </c>
       <c r="I31" t="n">
         <v>5.75</v>
       </c>
       <c r="J31" t="n">
-        <v>5.462626142520645</v>
+        <v>5.464103133510728</v>
       </c>
       <c r="K31" t="n">
         <v>5.6</v>
       </c>
       <c r="L31" t="n">
-        <v>6.460427263231642</v>
+        <v>6.321441899474546</v>
       </c>
     </row>
     <row r="32">
@@ -1640,37 +1640,37 @@
         <v>8.6</v>
       </c>
       <c r="B32" t="n">
-        <v>7.418004131136459</v>
+        <v>7.873955705577137</v>
       </c>
       <c r="C32" t="n">
         <v>7.5</v>
       </c>
       <c r="D32" t="n">
-        <v>8.230570760892158</v>
+        <v>7.877889864249218</v>
       </c>
       <c r="E32" t="n">
         <v>7</v>
       </c>
       <c r="F32" t="n">
-        <v>7.789820507658583</v>
+        <v>7.929633995419221</v>
       </c>
       <c r="G32" t="n">
         <v>7.25</v>
       </c>
       <c r="H32" t="n">
-        <v>6.903039459044558</v>
+        <v>7.541122366599593</v>
       </c>
       <c r="I32" t="n">
         <v>6.5</v>
       </c>
       <c r="J32" t="n">
-        <v>4.967690558692946</v>
+        <v>4.773049557075973</v>
       </c>
       <c r="K32" t="n">
         <v>7.4</v>
       </c>
       <c r="L32" t="n">
-        <v>7.559139940468685</v>
+        <v>7.237984447814593</v>
       </c>
     </row>
     <row r="33">
@@ -1678,37 +1678,37 @@
         <v>9.199999999999999</v>
       </c>
       <c r="B33" t="n">
-        <v>8.40821331514868</v>
+        <v>8.842713768211116</v>
       </c>
       <c r="C33" t="n">
         <v>9.25</v>
       </c>
       <c r="D33" t="n">
-        <v>9.100081214814796</v>
+        <v>8.821266523082425</v>
       </c>
       <c r="E33" t="n">
         <v>8.75</v>
       </c>
       <c r="F33" t="n">
-        <v>8.149352810622036</v>
+        <v>8.304612675655832</v>
       </c>
       <c r="G33" t="n">
         <v>8.25</v>
       </c>
       <c r="H33" t="n">
-        <v>7.783445983633217</v>
+        <v>8.404552601459468</v>
       </c>
       <c r="I33" t="n">
         <v>7.5</v>
       </c>
       <c r="J33" t="n">
-        <v>7.822840472471188</v>
+        <v>7.493939654590335</v>
       </c>
       <c r="K33" t="n">
         <v>7.8</v>
       </c>
       <c r="L33" t="n">
-        <v>7.907278427710054</v>
+        <v>7.493603689931136</v>
       </c>
     </row>
     <row r="34">
@@ -1716,37 +1716,37 @@
         <v>8.199999999999999</v>
       </c>
       <c r="B34" t="n">
-        <v>6.195819673522478</v>
+        <v>6.76154289254456</v>
       </c>
       <c r="C34" t="n">
         <v>6.5</v>
       </c>
       <c r="D34" t="n">
-        <v>7.535161064426534</v>
+        <v>7.193766283359625</v>
       </c>
       <c r="E34" t="n">
         <v>7</v>
       </c>
       <c r="F34" t="n">
-        <v>5.413503875053511</v>
+        <v>4.893770310254757</v>
       </c>
       <c r="G34" t="n">
         <v>8.5</v>
       </c>
       <c r="H34" t="n">
-        <v>5.413276409713919</v>
+        <v>5.986787120375486</v>
       </c>
       <c r="I34" t="n">
         <v>6</v>
       </c>
       <c r="J34" t="n">
-        <v>5.208816201599725</v>
+        <v>5.341945548138542</v>
       </c>
       <c r="K34" t="n">
         <v>3.4</v>
       </c>
       <c r="L34" t="n">
-        <v>4.414885704071291</v>
+        <v>4.475271399857363</v>
       </c>
     </row>
     <row r="35">
@@ -1754,37 +1754,37 @@
         <v>8.4</v>
       </c>
       <c r="B35" t="n">
-        <v>6.437797026308104</v>
+        <v>7.026792715120909</v>
       </c>
       <c r="C35" t="n">
         <v>8.5</v>
       </c>
       <c r="D35" t="n">
-        <v>7.898968495731498</v>
+        <v>7.566173478079432</v>
       </c>
       <c r="E35" t="n">
         <v>8</v>
       </c>
       <c r="F35" t="n">
-        <v>5.734887631582196</v>
+        <v>5.375286228518328</v>
       </c>
       <c r="G35" t="n">
         <v>6.5</v>
       </c>
       <c r="H35" t="n">
-        <v>5.554811753427789</v>
+        <v>6.121113100456617</v>
       </c>
       <c r="I35" t="n">
         <v>4.5</v>
       </c>
       <c r="J35" t="n">
-        <v>5.874826406047204</v>
+        <v>5.930897889433647</v>
       </c>
       <c r="K35" t="n">
         <v>5.8</v>
       </c>
       <c r="L35" t="n">
-        <v>4.925178699536775</v>
+        <v>4.962017529702559</v>
       </c>
     </row>
     <row r="36">
@@ -1792,37 +1792,37 @@
         <v>6.6</v>
       </c>
       <c r="B36" t="n">
-        <v>7.174054909715123</v>
+        <v>7.682823052805356</v>
       </c>
       <c r="C36" t="n">
         <v>6.75</v>
       </c>
       <c r="D36" t="n">
-        <v>8.202847014447354</v>
+        <v>7.946277879633235</v>
       </c>
       <c r="E36" t="n">
         <v>5.5</v>
       </c>
       <c r="F36" t="n">
-        <v>7.237019285275777</v>
+        <v>7.196486657484383</v>
       </c>
       <c r="G36" t="n">
         <v>5.25</v>
       </c>
       <c r="H36" t="n">
-        <v>6.240150476227877</v>
+        <v>6.832960200881931</v>
       </c>
       <c r="I36" t="n">
         <v>4.75</v>
       </c>
       <c r="J36" t="n">
-        <v>5.636986210441811</v>
+        <v>5.626301177364811</v>
       </c>
       <c r="K36" t="n">
         <v>4.8</v>
       </c>
       <c r="L36" t="n">
-        <v>6.092310559539635</v>
+        <v>5.886253489525341</v>
       </c>
     </row>
     <row r="37">
@@ -1830,37 +1830,37 @@
         <v>8.199999999999999</v>
       </c>
       <c r="B37" t="n">
-        <v>7.036777466188141</v>
+        <v>7.614325777736474</v>
       </c>
       <c r="C37" t="n">
         <v>7.5</v>
       </c>
       <c r="D37" t="n">
-        <v>7.91089155178303</v>
+        <v>7.643063402284749</v>
       </c>
       <c r="E37" t="n">
         <v>6.75</v>
       </c>
       <c r="F37" t="n">
-        <v>6.647346577315516</v>
+        <v>6.552039604156311</v>
       </c>
       <c r="G37" t="n">
         <v>7.5</v>
       </c>
       <c r="H37" t="n">
-        <v>6.846913798690029</v>
+        <v>7.50384732451837</v>
       </c>
       <c r="I37" t="n">
         <v>5.25</v>
       </c>
       <c r="J37" t="n">
-        <v>5.101837874262466</v>
+        <v>5.193902404102496</v>
       </c>
       <c r="K37" t="n">
         <v>4.8</v>
       </c>
       <c r="L37" t="n">
-        <v>6.898721039507395</v>
+        <v>6.785192878371936</v>
       </c>
     </row>
     <row r="38">
@@ -1868,37 +1868,37 @@
         <v>9</v>
       </c>
       <c r="B38" t="n">
-        <v>7.872994210831444</v>
+        <v>8.354635197822567</v>
       </c>
       <c r="C38" t="n">
         <v>8.25</v>
       </c>
       <c r="D38" t="n">
-        <v>9.064412507874703</v>
+        <v>8.829309937373276</v>
       </c>
       <c r="E38" t="n">
         <v>8.25</v>
       </c>
       <c r="F38" t="n">
-        <v>7.977546551213944</v>
+        <v>8.167539433782405</v>
       </c>
       <c r="G38" t="n">
         <v>8.5</v>
       </c>
       <c r="H38" t="n">
-        <v>7.113816305971405</v>
+        <v>7.796592932809312</v>
       </c>
       <c r="I38" t="n">
         <v>6</v>
       </c>
       <c r="J38" t="n">
-        <v>5.645383773643888</v>
+        <v>5.582764029637483</v>
       </c>
       <c r="K38" t="n">
         <v>6.4</v>
       </c>
       <c r="L38" t="n">
-        <v>6.635666759316157</v>
+        <v>6.492941585090374</v>
       </c>
     </row>
     <row r="39">
@@ -1906,37 +1906,37 @@
         <v>7.6</v>
       </c>
       <c r="B39" t="n">
-        <v>7.468331457226923</v>
+        <v>7.921782273217287</v>
       </c>
       <c r="C39" t="n">
         <v>9</v>
       </c>
       <c r="D39" t="n">
-        <v>8.61172054089301</v>
+        <v>8.264578207535685</v>
       </c>
       <c r="E39" t="n">
         <v>7.5</v>
       </c>
       <c r="F39" t="n">
-        <v>6.699817301548162</v>
+        <v>6.50312835670894</v>
       </c>
       <c r="G39" t="n">
         <v>7.5</v>
       </c>
       <c r="H39" t="n">
-        <v>6.551397973779749</v>
+        <v>7.155876172565253</v>
       </c>
       <c r="I39" t="n">
         <v>7.5</v>
       </c>
       <c r="J39" t="n">
-        <v>5.771693600547957</v>
+        <v>5.683658058420606</v>
       </c>
       <c r="K39" t="n">
         <v>5.2</v>
       </c>
       <c r="L39" t="n">
-        <v>4.836208139235269</v>
+        <v>4.777305673314284</v>
       </c>
     </row>
     <row r="40">
@@ -1944,37 +1944,37 @@
         <v>9</v>
       </c>
       <c r="B40" t="n">
-        <v>8.404808315170966</v>
+        <v>8.845419400661356</v>
       </c>
       <c r="C40" t="n">
         <v>8.5</v>
       </c>
       <c r="D40" t="n">
-        <v>9.027873153997739</v>
+        <v>8.759142918794407</v>
       </c>
       <c r="E40" t="n">
         <v>8</v>
       </c>
       <c r="F40" t="n">
-        <v>8.053980852430586</v>
+        <v>8.130743585606279</v>
       </c>
       <c r="G40" t="n">
         <v>7.75</v>
       </c>
       <c r="H40" t="n">
-        <v>7.515501177160367</v>
+        <v>8.130401972079069</v>
       </c>
       <c r="I40" t="n">
         <v>8</v>
       </c>
       <c r="J40" t="n">
-        <v>7.167243194198072</v>
+        <v>6.906748536711888</v>
       </c>
       <c r="K40" t="n">
         <v>6.8</v>
       </c>
       <c r="L40" t="n">
-        <v>7.316405922308912</v>
+        <v>6.976341525509243</v>
       </c>
     </row>
     <row r="41">
@@ -1982,37 +1982,37 @@
         <v>7.2</v>
       </c>
       <c r="B41" t="n">
-        <v>6.399600769546312</v>
+        <v>7.01483496497734</v>
       </c>
       <c r="C41" t="n">
         <v>7.25</v>
       </c>
       <c r="D41" t="n">
-        <v>7.16368586246496</v>
+        <v>6.79033428440045</v>
       </c>
       <c r="E41" t="n">
         <v>6</v>
       </c>
       <c r="F41" t="n">
-        <v>5.347776910238295</v>
+        <v>4.817066743522212</v>
       </c>
       <c r="G41" t="n">
         <v>5.75</v>
       </c>
       <c r="H41" t="n">
-        <v>6.09670788059631</v>
+        <v>6.664180465609037</v>
       </c>
       <c r="I41" t="n">
         <v>5</v>
       </c>
       <c r="J41" t="n">
-        <v>5.78009502067029</v>
+        <v>5.968368008437123</v>
       </c>
       <c r="K41" t="n">
         <v>7.4</v>
       </c>
       <c r="L41" t="n">
-        <v>6.750987027479511</v>
+        <v>6.632131296638557</v>
       </c>
     </row>
     <row r="42">
@@ -2020,37 +2020,37 @@
         <v>8.4</v>
       </c>
       <c r="B42" t="n">
-        <v>7.405396217139753</v>
+        <v>7.915363886895308</v>
       </c>
       <c r="C42" t="n">
         <v>6.75</v>
       </c>
       <c r="D42" t="n">
-        <v>7.192926236495364</v>
+        <v>6.65969240993549</v>
       </c>
       <c r="E42" t="n">
         <v>5.75</v>
       </c>
       <c r="F42" t="n">
-        <v>6.321739820714696</v>
+        <v>5.933976524323773</v>
       </c>
       <c r="G42" t="n">
         <v>8.25</v>
       </c>
       <c r="H42" t="n">
-        <v>7.016079578448002</v>
+        <v>7.575212031199963</v>
       </c>
       <c r="I42" t="n">
         <v>7.5</v>
       </c>
       <c r="J42" t="n">
-        <v>6.584969962612084</v>
+        <v>6.634706024770551</v>
       </c>
       <c r="K42" t="n">
         <v>6.8</v>
       </c>
       <c r="L42" t="n">
-        <v>6.578335125802802</v>
+        <v>6.382211751163647</v>
       </c>
     </row>
     <row r="43">
@@ -2058,37 +2058,37 @@
         <v>7.2</v>
       </c>
       <c r="B43" t="n">
-        <v>6.314161286231113</v>
+        <v>6.825252023856948</v>
       </c>
       <c r="C43" t="n">
         <v>6</v>
       </c>
       <c r="D43" t="n">
-        <v>6.702578430533126</v>
+        <v>6.228840056625047</v>
       </c>
       <c r="E43" t="n">
         <v>5.25</v>
       </c>
       <c r="F43" t="n">
-        <v>5.835226803979898</v>
+        <v>5.389945479052173</v>
       </c>
       <c r="G43" t="n">
         <v>6.75</v>
       </c>
       <c r="H43" t="n">
-        <v>6.902336992522589</v>
+        <v>7.47531530077372</v>
       </c>
       <c r="I43" t="n">
         <v>3.75</v>
       </c>
       <c r="J43" t="n">
-        <v>4.798559519094715</v>
+        <v>4.878742565457278</v>
       </c>
       <c r="K43" t="n">
         <v>7.4</v>
       </c>
       <c r="L43" t="n">
-        <v>7.003922839764169</v>
+        <v>6.900379365100862</v>
       </c>
     </row>
     <row r="44">
@@ -2096,37 +2096,37 @@
         <v>9</v>
       </c>
       <c r="B44" t="n">
-        <v>7.933508887693951</v>
+        <v>8.429206624955931</v>
       </c>
       <c r="C44" t="n">
         <v>9.5</v>
       </c>
       <c r="D44" t="n">
-        <v>8.892774932900023</v>
+        <v>8.610561187458964</v>
       </c>
       <c r="E44" t="n">
         <v>7.25</v>
       </c>
       <c r="F44" t="n">
-        <v>7.685455607973013</v>
+        <v>7.728226810032312</v>
       </c>
       <c r="G44" t="n">
         <v>8.25</v>
       </c>
       <c r="H44" t="n">
-        <v>7.048689404989834</v>
+        <v>7.651094276993386</v>
       </c>
       <c r="I44" t="n">
         <v>6.5</v>
       </c>
       <c r="J44" t="n">
-        <v>7.112579706572887</v>
+        <v>6.996408786300904</v>
       </c>
       <c r="K44" t="n">
         <v>5.8</v>
       </c>
       <c r="L44" t="n">
-        <v>6.407320140829122</v>
+        <v>6.21121531194799</v>
       </c>
     </row>
     <row r="45">
@@ -2134,37 +2134,37 @@
         <v>6.6</v>
       </c>
       <c r="B45" t="n">
-        <v>8.022549044161899</v>
+        <v>8.474812563943669</v>
       </c>
       <c r="C45" t="n">
         <v>7.75</v>
       </c>
       <c r="D45" t="n">
-        <v>7.251205773707559</v>
+        <v>6.807794990342889</v>
       </c>
       <c r="E45" t="n">
         <v>5</v>
       </c>
       <c r="F45" t="n">
-        <v>7.373347090067835</v>
+        <v>7.262181044833771</v>
       </c>
       <c r="G45" t="n">
         <v>6.25</v>
       </c>
       <c r="H45" t="n">
-        <v>7.593485658523946</v>
+        <v>8.162751313358537</v>
       </c>
       <c r="I45" t="n">
         <v>6.75</v>
       </c>
       <c r="J45" t="n">
-        <v>6.398255365208106</v>
+        <v>6.370270547648264</v>
       </c>
       <c r="K45" t="n">
         <v>6.2</v>
       </c>
       <c r="L45" t="n">
-        <v>6.556103416375136</v>
+        <v>6.26626498758232</v>
       </c>
     </row>
     <row r="46">
@@ -2172,37 +2172,37 @@
         <v>8</v>
       </c>
       <c r="B46" t="n">
-        <v>6.22625050717334</v>
+        <v>6.830242341842702</v>
       </c>
       <c r="C46" t="n">
         <v>8.5</v>
       </c>
       <c r="D46" t="n">
-        <v>6.481425404395716</v>
+        <v>5.976253370155801</v>
       </c>
       <c r="E46" t="n">
         <v>7.75</v>
       </c>
       <c r="F46" t="n">
-        <v>5.927409627823828</v>
+        <v>5.621197587317982</v>
       </c>
       <c r="G46" t="n">
         <v>7.75</v>
       </c>
       <c r="H46" t="n">
-        <v>6.53725676556345</v>
+        <v>7.129043413189601</v>
       </c>
       <c r="I46" t="n">
         <v>3.75</v>
       </c>
       <c r="J46" t="n">
-        <v>5.220288956401486</v>
+        <v>5.440782143640695</v>
       </c>
       <c r="K46" t="n">
         <v>6</v>
       </c>
       <c r="L46" t="n">
-        <v>5.68908325533955</v>
+        <v>5.747240067161089</v>
       </c>
     </row>
     <row r="47">
@@ -2210,37 +2210,37 @@
         <v>8.199999999999999</v>
       </c>
       <c r="B47" t="n">
-        <v>7.421331240228305</v>
+        <v>7.937746349808921</v>
       </c>
       <c r="C47" t="n">
         <v>7</v>
       </c>
       <c r="D47" t="n">
-        <v>7.786107807126186</v>
+        <v>7.396639587059572</v>
       </c>
       <c r="E47" t="n">
         <v>6</v>
       </c>
       <c r="F47" t="n">
-        <v>6.686452744399298</v>
+        <v>6.391828850943799</v>
       </c>
       <c r="G47" t="n">
         <v>7.5</v>
       </c>
       <c r="H47" t="n">
-        <v>6.88115236979643</v>
+        <v>7.461157324324838</v>
       </c>
       <c r="I47" t="n">
         <v>5</v>
       </c>
       <c r="J47" t="n">
-        <v>5.25490844469843</v>
+        <v>5.29816001753923</v>
       </c>
       <c r="K47" t="n">
         <v>9.199999999999999</v>
       </c>
       <c r="L47" t="n">
-        <v>7.318326476566616</v>
+        <v>7.160845890048666</v>
       </c>
     </row>
     <row r="48">
@@ -2248,37 +2248,37 @@
         <v>7.8</v>
       </c>
       <c r="B48" t="n">
-        <v>7.394767094797828</v>
+        <v>7.880154773387421</v>
       </c>
       <c r="C48" t="n">
         <v>7.25</v>
       </c>
       <c r="D48" t="n">
-        <v>8.182166573231036</v>
+        <v>7.808608122050409</v>
       </c>
       <c r="E48" t="n">
         <v>7.25</v>
       </c>
       <c r="F48" t="n">
-        <v>7.023435293558664</v>
+        <v>6.836814795744531</v>
       </c>
       <c r="G48" t="n">
         <v>7.5</v>
       </c>
       <c r="H48" t="n">
-        <v>7.094221399814386</v>
+        <v>7.683214663507309</v>
       </c>
       <c r="I48" t="n">
         <v>5.5</v>
       </c>
       <c r="J48" t="n">
-        <v>5.931812231927927</v>
+        <v>5.796679745801754</v>
       </c>
       <c r="K48" t="n">
         <v>5.4</v>
       </c>
       <c r="L48" t="n">
-        <v>6.050021192572661</v>
+        <v>5.858091265630819</v>
       </c>
     </row>
     <row r="49">
@@ -2286,37 +2286,37 @@
         <v>8.6</v>
       </c>
       <c r="B49" t="n">
-        <v>8.147577599886858</v>
+        <v>8.613219367325566</v>
       </c>
       <c r="C49" t="n">
         <v>7.75</v>
       </c>
       <c r="D49" t="n">
-        <v>8.596166004123429</v>
+        <v>8.301887875292412</v>
       </c>
       <c r="E49" t="n">
         <v>6.75</v>
       </c>
       <c r="F49" t="n">
-        <v>7.78000787596048</v>
+        <v>7.821439922108671</v>
       </c>
       <c r="G49" t="n">
         <v>7.75</v>
       </c>
       <c r="H49" t="n">
-        <v>7.957435528425068</v>
+        <v>8.545312344071574</v>
       </c>
       <c r="I49" t="n">
         <v>8</v>
       </c>
       <c r="J49" t="n">
-        <v>7.057690467127597</v>
+        <v>6.805544457554593</v>
       </c>
       <c r="K49" t="n">
         <v>5.6</v>
       </c>
       <c r="L49" t="n">
-        <v>5.95168551646699</v>
+        <v>5.707739928774409</v>
       </c>
     </row>
     <row r="50">
@@ -2324,37 +2324,37 @@
         <v>7.8</v>
       </c>
       <c r="B50" t="n">
-        <v>7.904702390778797</v>
+        <v>8.377606525755496</v>
       </c>
       <c r="C50" t="n">
         <v>7.75</v>
       </c>
       <c r="D50" t="n">
-        <v>8.401711612287048</v>
+        <v>8.035170893383572</v>
       </c>
       <c r="E50" t="n">
         <v>7.5</v>
       </c>
       <c r="F50" t="n">
-        <v>7.42419406900742</v>
+        <v>7.321351218870283</v>
       </c>
       <c r="G50" t="n">
         <v>8</v>
       </c>
       <c r="H50" t="n">
-        <v>7.516896263960824</v>
+        <v>8.104873559983456</v>
       </c>
       <c r="I50" t="n">
         <v>6.25</v>
       </c>
       <c r="J50" t="n">
-        <v>7.027901071816365</v>
+        <v>6.789070730388417</v>
       </c>
       <c r="K50" t="n">
         <v>8.199999999999999</v>
       </c>
       <c r="L50" t="n">
-        <v>8.297100870173979</v>
+        <v>7.971169811412283</v>
       </c>
     </row>
     <row r="51">
@@ -2362,37 +2362,37 @@
         <v>8.4</v>
       </c>
       <c r="B51" t="n">
-        <v>7.519578158154816</v>
+        <v>8.011077252602028</v>
       </c>
       <c r="C51" t="n">
         <v>8</v>
       </c>
       <c r="D51" t="n">
-        <v>8.573578829592776</v>
+        <v>8.225095892056375</v>
       </c>
       <c r="E51" t="n">
         <v>6.25</v>
       </c>
       <c r="F51" t="n">
-        <v>6.313710119357896</v>
+        <v>5.878003147099708</v>
       </c>
       <c r="G51" t="n">
         <v>7.5</v>
       </c>
       <c r="H51" t="n">
-        <v>6.428449050340392</v>
+        <v>6.970285182362399</v>
       </c>
       <c r="I51" t="n">
         <v>6</v>
       </c>
       <c r="J51" t="n">
-        <v>6.713994500335899</v>
+        <v>6.618858410820112</v>
       </c>
       <c r="K51" t="n">
         <v>7</v>
       </c>
       <c r="L51" t="n">
-        <v>6.643681015211326</v>
+        <v>6.494072068271691</v>
       </c>
     </row>
     <row r="52">
@@ -2400,37 +2400,37 @@
         <v>4.6</v>
       </c>
       <c r="B52" t="n">
-        <v>6.203233330081632</v>
+        <v>6.808127716521588</v>
       </c>
       <c r="C52" t="n">
         <v>7.5</v>
       </c>
       <c r="D52" t="n">
-        <v>7.481608934329463</v>
+        <v>7.092332228102999</v>
       </c>
       <c r="E52" t="n">
         <v>4.5</v>
       </c>
       <c r="F52" t="n">
-        <v>5.283934439580882</v>
+        <v>4.680318980312339</v>
       </c>
       <c r="G52" t="n">
         <v>7</v>
       </c>
       <c r="H52" t="n">
-        <v>5.894387900162023</v>
+        <v>6.47405491967916</v>
       </c>
       <c r="I52" t="n">
         <v>5</v>
       </c>
       <c r="J52" t="n">
-        <v>5.322459955289085</v>
+        <v>5.604562769533925</v>
       </c>
       <c r="K52" t="n">
         <v>3.2</v>
       </c>
       <c r="L52" t="n">
-        <v>4.945431329127137</v>
+        <v>5.100625199591907</v>
       </c>
     </row>
     <row r="53">
@@ -2438,37 +2438,37 @@
         <v>8.800000000000001</v>
       </c>
       <c r="B53" t="n">
-        <v>7.658815059430903</v>
+        <v>8.189209507456761</v>
       </c>
       <c r="C53" t="n">
         <v>6.75</v>
       </c>
       <c r="D53" t="n">
-        <v>7.639532046030197</v>
+        <v>7.228055203638252</v>
       </c>
       <c r="E53" t="n">
         <v>7.5</v>
       </c>
       <c r="F53" t="n">
-        <v>6.722121119836386</v>
+        <v>6.531446965246363</v>
       </c>
       <c r="G53" t="n">
         <v>6.75</v>
       </c>
       <c r="H53" t="n">
-        <v>6.723330473824505</v>
+        <v>7.238923743591485</v>
       </c>
       <c r="I53" t="n">
         <v>7.5</v>
       </c>
       <c r="J53" t="n">
-        <v>6.85353388042312</v>
+        <v>6.848247194025063</v>
       </c>
       <c r="K53" t="n">
         <v>5</v>
       </c>
       <c r="L53" t="n">
-        <v>4.744511488396632</v>
+        <v>4.666383501064621</v>
       </c>
     </row>
     <row r="54">
@@ -2476,37 +2476,37 @@
         <v>7.6</v>
       </c>
       <c r="B54" t="n">
-        <v>6.752896072567445</v>
+        <v>7.257037538198968</v>
       </c>
       <c r="C54" t="n">
         <v>8</v>
       </c>
       <c r="D54" t="n">
-        <v>7.400381680509996</v>
+        <v>6.953053206779101</v>
       </c>
       <c r="E54" t="n">
         <v>5.75</v>
       </c>
       <c r="F54" t="n">
-        <v>5.112428479902251</v>
+        <v>4.353260232645078</v>
       </c>
       <c r="G54" t="n">
         <v>7.75</v>
       </c>
       <c r="H54" t="n">
-        <v>6.322528942949891</v>
+        <v>6.904644859175417</v>
       </c>
       <c r="I54" t="n">
         <v>3.5</v>
       </c>
       <c r="J54" t="n">
-        <v>5.266832947790791</v>
+        <v>5.312830642702991</v>
       </c>
       <c r="K54" t="n">
         <v>7.2</v>
       </c>
       <c r="L54" t="n">
-        <v>5.541326308291077</v>
+        <v>5.573757605205115</v>
       </c>
     </row>
     <row r="55">
@@ -2514,37 +2514,37 @@
         <v>8.4</v>
       </c>
       <c r="B55" t="n">
-        <v>7.642054302586564</v>
+        <v>8.106944124663466</v>
       </c>
       <c r="C55" t="n">
         <v>9.5</v>
       </c>
       <c r="D55" t="n">
-        <v>8.864454494142562</v>
+        <v>8.590147242561608</v>
       </c>
       <c r="E55" t="n">
         <v>7.5</v>
       </c>
       <c r="F55" t="n">
-        <v>7.195317283023633</v>
+        <v>7.135074519981067</v>
       </c>
       <c r="G55" t="n">
         <v>7.75</v>
       </c>
       <c r="H55" t="n">
-        <v>7.274485396541378</v>
+        <v>7.932845418474574</v>
       </c>
       <c r="I55" t="n">
         <v>7</v>
       </c>
       <c r="J55" t="n">
-        <v>5.833586767441665</v>
+        <v>5.729692915736281</v>
       </c>
       <c r="K55" t="n">
         <v>8</v>
       </c>
       <c r="L55" t="n">
-        <v>7.370495470922371</v>
+        <v>7.233430681012786</v>
       </c>
     </row>
     <row r="56">
@@ -2552,37 +2552,37 @@
         <v>6</v>
       </c>
       <c r="B56" t="n">
-        <v>6.092833397517346</v>
+        <v>6.695122291284267</v>
       </c>
       <c r="C56" t="n">
         <v>6</v>
       </c>
       <c r="D56" t="n">
-        <v>6.873801023264935</v>
+        <v>6.426219957555001</v>
       </c>
       <c r="E56" t="n">
         <v>4.75</v>
       </c>
       <c r="F56" t="n">
-        <v>5.289824585395362</v>
+        <v>4.693127086358094</v>
       </c>
       <c r="G56" t="n">
         <v>6.5</v>
       </c>
       <c r="H56" t="n">
-        <v>6.067951552048847</v>
+        <v>6.592379199387691</v>
       </c>
       <c r="I56" t="n">
         <v>5.25</v>
       </c>
       <c r="J56" t="n">
-        <v>4.152019163047058</v>
+        <v>4.364134907850415</v>
       </c>
       <c r="K56" t="n">
         <v>4</v>
       </c>
       <c r="L56" t="n">
-        <v>4.068804382194051</v>
+        <v>4.11311262423819</v>
       </c>
     </row>
     <row r="57">
@@ -2590,37 +2590,37 @@
         <v>7.8</v>
       </c>
       <c r="B57" t="n">
-        <v>6.838489615889308</v>
+        <v>7.372694447207608</v>
       </c>
       <c r="C57" t="n">
         <v>8</v>
       </c>
       <c r="D57" t="n">
-        <v>7.382315287495408</v>
+        <v>6.978153636075543</v>
       </c>
       <c r="E57" t="n">
         <v>6.75</v>
       </c>
       <c r="F57" t="n">
-        <v>6.628051237844762</v>
+        <v>6.431612330395738</v>
       </c>
       <c r="G57" t="n">
         <v>7.5</v>
       </c>
       <c r="H57" t="n">
-        <v>7.143801269930415</v>
+        <v>7.711424050661276</v>
       </c>
       <c r="I57" t="n">
         <v>6.75</v>
       </c>
       <c r="J57" t="n">
-        <v>4.027638283932181</v>
+        <v>3.961836713734868</v>
       </c>
       <c r="K57" t="n">
         <v>5</v>
       </c>
       <c r="L57" t="n">
-        <v>5.051266593317965</v>
+        <v>5.064088698473309</v>
       </c>
     </row>
     <row r="58">
@@ -2628,37 +2628,37 @@
         <v>8.6</v>
       </c>
       <c r="B58" t="n">
-        <v>8.282049227607084</v>
+        <v>8.712695699440822</v>
       </c>
       <c r="C58" t="n">
         <v>7.75</v>
       </c>
       <c r="D58" t="n">
-        <v>8.823303170795661</v>
+        <v>8.495277271251432</v>
       </c>
       <c r="E58" t="n">
         <v>8.25</v>
       </c>
       <c r="F58" t="n">
-        <v>8.113544136402462</v>
+        <v>8.269398050913594</v>
       </c>
       <c r="G58" t="n">
         <v>8.75</v>
       </c>
       <c r="H58" t="n">
-        <v>7.568954748493185</v>
+        <v>8.184690090242068</v>
       </c>
       <c r="I58" t="n">
         <v>7</v>
       </c>
       <c r="J58" t="n">
-        <v>7.031628799363514</v>
+        <v>6.699045837227549</v>
       </c>
       <c r="K58" t="n">
         <v>8.4</v>
       </c>
       <c r="L58" t="n">
-        <v>7.955819195828746</v>
+        <v>7.552361111348395</v>
       </c>
     </row>
     <row r="59">
@@ -2666,37 +2666,37 @@
         <v>8.6</v>
       </c>
       <c r="B59" t="n">
-        <v>8.294158810360479</v>
+        <v>8.72899242329839</v>
       </c>
       <c r="C59" t="n">
         <v>8.25</v>
       </c>
       <c r="D59" t="n">
-        <v>8.765755797618262</v>
+        <v>8.39560268653071</v>
       </c>
       <c r="E59" t="n">
         <v>8.25</v>
       </c>
       <c r="F59" t="n">
-        <v>8.499810456700564</v>
+        <v>8.786641801978202</v>
       </c>
       <c r="G59" t="n">
         <v>8.25</v>
       </c>
       <c r="H59" t="n">
-        <v>8.121761361932235</v>
+        <v>8.697458376676543</v>
       </c>
       <c r="I59" t="n">
         <v>7</v>
       </c>
       <c r="J59" t="n">
-        <v>6.777518872263922</v>
+        <v>6.402496045214945</v>
       </c>
       <c r="K59" t="n">
         <v>7.4</v>
       </c>
       <c r="L59" t="n">
-        <v>8.322275408848769</v>
+        <v>7.840390656634593</v>
       </c>
     </row>
     <row r="60">
@@ -2704,37 +2704,37 @@
         <v>7.2</v>
       </c>
       <c r="B60" t="n">
-        <v>6.617656641238212</v>
+        <v>7.231826182822132</v>
       </c>
       <c r="C60" t="n">
         <v>6.25</v>
       </c>
       <c r="D60" t="n">
-        <v>7.749386564438494</v>
+        <v>7.416149436285233</v>
       </c>
       <c r="E60" t="n">
         <v>5.75</v>
       </c>
       <c r="F60" t="n">
-        <v>5.992873535995559</v>
+        <v>5.722476509710734</v>
       </c>
       <c r="G60" t="n">
         <v>7</v>
       </c>
       <c r="H60" t="n">
-        <v>7.353997087634774</v>
+        <v>7.969440541258896</v>
       </c>
       <c r="I60" t="n">
         <v>5.25</v>
       </c>
       <c r="J60" t="n">
-        <v>6.846697347111264</v>
+        <v>6.868940152794174</v>
       </c>
       <c r="K60" t="n">
         <v>6.2</v>
       </c>
       <c r="L60" t="n">
-        <v>5.171927734539584</v>
+        <v>5.207359206546916</v>
       </c>
     </row>
     <row r="61">
@@ -2742,37 +2742,37 @@
         <v>7.4</v>
       </c>
       <c r="B61" t="n">
-        <v>6.929785339709144</v>
+        <v>7.463391264985629</v>
       </c>
       <c r="C61" t="n">
         <v>8.5</v>
       </c>
       <c r="D61" t="n">
-        <v>7.979327211527766</v>
+        <v>7.608102452185133</v>
       </c>
       <c r="E61" t="n">
         <v>4.5</v>
       </c>
       <c r="F61" t="n">
-        <v>5.71111317137446</v>
+        <v>5.202956089297232</v>
       </c>
       <c r="G61" t="n">
         <v>8.25</v>
       </c>
       <c r="H61" t="n">
-        <v>5.933265373903589</v>
+        <v>6.428664077292908</v>
       </c>
       <c r="I61" t="n">
         <v>7.25</v>
       </c>
       <c r="J61" t="n">
-        <v>6.486187447629687</v>
+        <v>6.520523923665529</v>
       </c>
       <c r="K61" t="n">
         <v>4.6</v>
       </c>
       <c r="L61" t="n">
-        <v>4.440159652104534</v>
+        <v>4.436071504448441</v>
       </c>
     </row>
     <row r="62">
@@ -2780,37 +2780,37 @@
         <v>7.6</v>
       </c>
       <c r="B62" t="n">
-        <v>7.194009352270761</v>
+        <v>7.69917891365011</v>
       </c>
       <c r="C62" t="n">
         <v>9</v>
       </c>
       <c r="D62" t="n">
-        <v>8.345344604844666</v>
+        <v>8.015762139515722</v>
       </c>
       <c r="E62" t="n">
         <v>7.5</v>
       </c>
       <c r="F62" t="n">
-        <v>6.540385845595593</v>
+        <v>6.306637132115532</v>
       </c>
       <c r="G62" t="n">
         <v>7.5</v>
       </c>
       <c r="H62" t="n">
-        <v>6.789188464081604</v>
+        <v>7.443327003655896</v>
       </c>
       <c r="I62" t="n">
         <v>7.5</v>
       </c>
       <c r="J62" t="n">
-        <v>6.509190425506286</v>
+        <v>6.437824929048448</v>
       </c>
       <c r="K62" t="n">
         <v>5.2</v>
       </c>
       <c r="L62" t="n">
-        <v>6.222014898888614</v>
+        <v>6.062591631784088</v>
       </c>
     </row>
     <row r="63">
@@ -2818,37 +2818,37 @@
         <v>7.6</v>
       </c>
       <c r="B63" t="n">
-        <v>7.260628795192958</v>
+        <v>7.766383814858729</v>
       </c>
       <c r="C63" t="n">
         <v>8.25</v>
       </c>
       <c r="D63" t="n">
-        <v>8.148521167728665</v>
+        <v>7.808390989841862</v>
       </c>
       <c r="E63" t="n">
         <v>8</v>
       </c>
       <c r="F63" t="n">
-        <v>6.487605961533001</v>
+        <v>6.143750784638979</v>
       </c>
       <c r="G63" t="n">
         <v>7.75</v>
       </c>
       <c r="H63" t="n">
-        <v>7.125404907247834</v>
+        <v>7.685265521287828</v>
       </c>
       <c r="I63" t="n">
         <v>5.5</v>
       </c>
       <c r="J63" t="n">
-        <v>6.125418678559199</v>
+        <v>6.104645838200313</v>
       </c>
       <c r="K63" t="n">
         <v>7.4</v>
       </c>
       <c r="L63" t="n">
-        <v>7.646087756033944</v>
+        <v>7.471927966017919</v>
       </c>
     </row>
     <row r="64">
@@ -2856,37 +2856,37 @@
         <v>7.4</v>
       </c>
       <c r="B64" t="n">
-        <v>7.162659825175106</v>
+        <v>7.795914336570048</v>
       </c>
       <c r="C64" t="n">
         <v>6.25</v>
       </c>
       <c r="D64" t="n">
-        <v>8.355364558113511</v>
+        <v>8.086476832438869</v>
       </c>
       <c r="E64" t="n">
         <v>6.25</v>
       </c>
       <c r="F64" t="n">
-        <v>7.141418741063461</v>
+        <v>7.211423127542919</v>
       </c>
       <c r="G64" t="n">
         <v>8</v>
       </c>
       <c r="H64" t="n">
-        <v>7.698973884887288</v>
+        <v>8.266124000176415</v>
       </c>
       <c r="I64" t="n">
         <v>6</v>
       </c>
       <c r="J64" t="n">
-        <v>7.413922600958231</v>
+        <v>7.363478826063819</v>
       </c>
       <c r="K64" t="n">
         <v>6.4</v>
       </c>
       <c r="L64" t="n">
-        <v>7.616485428246929</v>
+        <v>7.349844800776852</v>
       </c>
     </row>
     <row r="65">
@@ -2894,37 +2894,37 @@
         <v>6.6</v>
       </c>
       <c r="B65" t="n">
-        <v>6.744485264460589</v>
+        <v>7.304309591147263</v>
       </c>
       <c r="C65" t="n">
         <v>7.25</v>
       </c>
       <c r="D65" t="n">
-        <v>7.854961463792535</v>
+        <v>7.505622182379395</v>
       </c>
       <c r="E65" t="n">
         <v>4</v>
       </c>
       <c r="F65" t="n">
-        <v>6.26872361541007</v>
+        <v>6.009712612877228</v>
       </c>
       <c r="G65" t="n">
         <v>7</v>
       </c>
       <c r="H65" t="n">
-        <v>6.390383598858828</v>
+        <v>7.024744382141932</v>
       </c>
       <c r="I65" t="n">
         <v>5</v>
       </c>
       <c r="J65" t="n">
-        <v>5.875795764161731</v>
+        <v>5.991383596420763</v>
       </c>
       <c r="K65" t="n">
         <v>4.8</v>
       </c>
       <c r="L65" t="n">
-        <v>6.638787741510311</v>
+        <v>6.577785001085253</v>
       </c>
     </row>
     <row r="66">
@@ -2932,37 +2932,37 @@
         <v>7.8</v>
       </c>
       <c r="B66" t="n">
-        <v>7.50700734454177</v>
+        <v>7.95425612602031</v>
       </c>
       <c r="C66" t="n">
         <v>9.25</v>
       </c>
       <c r="D66" t="n">
-        <v>8.547957623013993</v>
+        <v>8.227840778777994</v>
       </c>
       <c r="E66" t="n">
         <v>8</v>
       </c>
       <c r="F66" t="n">
-        <v>7.63430912843543</v>
+        <v>7.734039334758875</v>
       </c>
       <c r="G66" t="n">
         <v>7.5</v>
       </c>
       <c r="H66" t="n">
-        <v>6.079976509305925</v>
+        <v>6.667358838845741</v>
       </c>
       <c r="I66" t="n">
         <v>6.25</v>
       </c>
       <c r="J66" t="n">
-        <v>4.9892767504742</v>
+        <v>4.855554660650744</v>
       </c>
       <c r="K66" t="n">
         <v>8.6</v>
       </c>
       <c r="L66" t="n">
-        <v>8.763253718823799</v>
+        <v>8.509377217941505</v>
       </c>
     </row>
     <row r="67">
@@ -2970,37 +2970,37 @@
         <v>7.6</v>
       </c>
       <c r="B67" t="n">
-        <v>6.599211785172888</v>
+        <v>7.228378646250373</v>
       </c>
       <c r="C67" t="n">
         <v>5.75</v>
       </c>
       <c r="D67" t="n">
-        <v>7.146789819943979</v>
+        <v>6.785954734883095</v>
       </c>
       <c r="E67" t="n">
         <v>5</v>
       </c>
       <c r="F67" t="n">
-        <v>6.099747701110291</v>
+        <v>5.906056299456579</v>
       </c>
       <c r="G67" t="n">
         <v>5.25</v>
       </c>
       <c r="H67" t="n">
-        <v>4.818848176539717</v>
+        <v>5.323767281308011</v>
       </c>
       <c r="I67" t="n">
         <v>3.5</v>
       </c>
       <c r="J67" t="n">
-        <v>4.322468451511943</v>
+        <v>4.544800439501113</v>
       </c>
       <c r="K67" t="n">
         <v>4.2</v>
       </c>
       <c r="L67" t="n">
-        <v>4.166449465253898</v>
+        <v>4.239207524493739</v>
       </c>
     </row>
     <row r="68">
@@ -3008,37 +3008,37 @@
         <v>7.8</v>
       </c>
       <c r="B68" t="n">
-        <v>7.621593500781825</v>
+        <v>8.144242170454511</v>
       </c>
       <c r="C68" t="n">
         <v>7.25</v>
       </c>
       <c r="D68" t="n">
-        <v>8.007010940705626</v>
+        <v>7.616227162775498</v>
       </c>
       <c r="E68" t="n">
         <v>6.5</v>
       </c>
       <c r="F68" t="n">
-        <v>6.962566190782852</v>
+        <v>6.795072630703618</v>
       </c>
       <c r="G68" t="n">
         <v>7.5</v>
       </c>
       <c r="H68" t="n">
-        <v>6.98006804988109</v>
+        <v>7.558716910503194</v>
       </c>
       <c r="I68" t="n">
         <v>5</v>
       </c>
       <c r="J68" t="n">
-        <v>5.846101715054335</v>
+        <v>5.822848802371345</v>
       </c>
       <c r="K68" t="n">
         <v>6.8</v>
       </c>
       <c r="L68" t="n">
-        <v>7.193613337540444</v>
+        <v>7.097657347829056</v>
       </c>
     </row>
     <row r="69">
@@ -3046,37 +3046,37 @@
         <v>7.4</v>
       </c>
       <c r="B69" t="n">
-        <v>6.7431890607936</v>
+        <v>7.37771805830814</v>
       </c>
       <c r="C69" t="n">
         <v>7.25</v>
       </c>
       <c r="D69" t="n">
-        <v>7.422251769775505</v>
+        <v>7.083009872663403</v>
       </c>
       <c r="E69" t="n">
         <v>4.5</v>
       </c>
       <c r="F69" t="n">
-        <v>6.549440082880304</v>
+        <v>6.472141949067479</v>
       </c>
       <c r="G69" t="n">
         <v>6.25</v>
       </c>
       <c r="H69" t="n">
-        <v>6.246483194641393</v>
+        <v>6.840988697983893</v>
       </c>
       <c r="I69" t="n">
         <v>4.25</v>
       </c>
       <c r="J69" t="n">
-        <v>5.320913370633124</v>
+        <v>5.42600566814688</v>
       </c>
       <c r="K69" t="n">
         <v>5.6</v>
       </c>
       <c r="L69" t="n">
-        <v>6.721611465125709</v>
+        <v>6.65708208161243</v>
       </c>
     </row>
     <row r="70">
@@ -3084,37 +3084,37 @@
         <v>8.4</v>
       </c>
       <c r="B70" t="n">
-        <v>6.944237116391886</v>
+        <v>7.448896357728112</v>
       </c>
       <c r="C70" t="n">
         <v>7.5</v>
       </c>
       <c r="D70" t="n">
-        <v>8.132610090654694</v>
+        <v>7.794931997172398</v>
       </c>
       <c r="E70" t="n">
         <v>6.25</v>
       </c>
       <c r="F70" t="n">
-        <v>6.389134703766755</v>
+        <v>6.052838971512866</v>
       </c>
       <c r="G70" t="n">
         <v>7.5</v>
       </c>
       <c r="H70" t="n">
-        <v>6.575541342877249</v>
+        <v>7.171531233943807</v>
       </c>
       <c r="I70" t="n">
         <v>5</v>
       </c>
       <c r="J70" t="n">
-        <v>3.712549322370372</v>
+        <v>3.68125982129489</v>
       </c>
       <c r="K70" t="n">
         <v>5.2</v>
       </c>
       <c r="L70" t="n">
-        <v>4.859043318267981</v>
+        <v>4.825797355432089</v>
       </c>
     </row>
     <row r="71">
@@ -3122,37 +3122,37 @@
         <v>7.8</v>
       </c>
       <c r="B71" t="n">
-        <v>7.468331457226923</v>
+        <v>7.921782273217287</v>
       </c>
       <c r="C71" t="n">
         <v>8.5</v>
       </c>
       <c r="D71" t="n">
-        <v>8.61172054089301</v>
+        <v>8.264578207535685</v>
       </c>
       <c r="E71" t="n">
         <v>7.5</v>
       </c>
       <c r="F71" t="n">
-        <v>6.699817301548162</v>
+        <v>6.50312835670894</v>
       </c>
       <c r="G71" t="n">
         <v>8.5</v>
       </c>
       <c r="H71" t="n">
-        <v>6.551397973779749</v>
+        <v>7.155876172565253</v>
       </c>
       <c r="I71" t="n">
         <v>6.25</v>
       </c>
       <c r="J71" t="n">
-        <v>5.771693600547957</v>
+        <v>5.683658058420606</v>
       </c>
       <c r="K71" t="n">
         <v>6</v>
       </c>
       <c r="L71" t="n">
-        <v>4.836208139235269</v>
+        <v>4.777305673314284</v>
       </c>
     </row>
     <row r="72">
@@ -3160,37 +3160,37 @@
         <v>6</v>
       </c>
       <c r="B72" t="n">
-        <v>6.702075937816444</v>
+        <v>7.242918983684342</v>
       </c>
       <c r="C72" t="n">
         <v>6.25</v>
       </c>
       <c r="D72" t="n">
-        <v>6.988502840208064</v>
+        <v>6.566991005714418</v>
       </c>
       <c r="E72" t="n">
         <v>4.75</v>
       </c>
       <c r="F72" t="n">
-        <v>5.875816937111914</v>
+        <v>5.468148628625119</v>
       </c>
       <c r="G72" t="n">
         <v>3.75</v>
       </c>
       <c r="H72" t="n">
-        <v>6.063377256045005</v>
+        <v>6.614451216221941</v>
       </c>
       <c r="I72" t="n">
         <v>5.25</v>
       </c>
       <c r="J72" t="n">
-        <v>4.290632385487183</v>
+        <v>4.297193232411649</v>
       </c>
       <c r="K72" t="n">
         <v>9.800000000000001</v>
       </c>
       <c r="L72" t="n">
-        <v>7.809260303790442</v>
+        <v>7.614380441666738</v>
       </c>
     </row>
     <row r="73">
@@ -3198,37 +3198,37 @@
         <v>7</v>
       </c>
       <c r="B73" t="n">
-        <v>7.338042270124697</v>
+        <v>7.92027218818873</v>
       </c>
       <c r="C73" t="n">
         <v>8.5</v>
       </c>
       <c r="D73" t="n">
-        <v>8.146777667941388</v>
+        <v>7.847024767285736</v>
       </c>
       <c r="E73" t="n">
         <v>6.5</v>
       </c>
       <c r="F73" t="n">
-        <v>7.010515633072202</v>
+        <v>6.942277198786125</v>
       </c>
       <c r="G73" t="n">
         <v>6.5</v>
       </c>
       <c r="H73" t="n">
-        <v>6.386474691199401</v>
+        <v>6.881605308922922</v>
       </c>
       <c r="I73" t="n">
         <v>5.5</v>
       </c>
       <c r="J73" t="n">
-        <v>5.234139535052982</v>
+        <v>5.218216928132926</v>
       </c>
       <c r="K73" t="n">
         <v>4.6</v>
       </c>
       <c r="L73" t="n">
-        <v>5.583062325150473</v>
+        <v>5.46758918664758</v>
       </c>
     </row>
     <row r="74">
@@ -3236,37 +3236,37 @@
         <v>7</v>
       </c>
       <c r="B74" t="n">
-        <v>6.973875310870009</v>
+        <v>7.485556684454981</v>
       </c>
       <c r="C74" t="n">
         <v>7.5</v>
       </c>
       <c r="D74" t="n">
-        <v>7.458283225361906</v>
+        <v>7.032251635708869</v>
       </c>
       <c r="E74" t="n">
         <v>6.75</v>
       </c>
       <c r="F74" t="n">
-        <v>7.260474466684721</v>
+        <v>7.252710643117619</v>
       </c>
       <c r="G74" t="n">
         <v>7.5</v>
       </c>
       <c r="H74" t="n">
-        <v>6.684891386442554</v>
+        <v>7.229399770091021</v>
       </c>
       <c r="I74" t="n">
         <v>6.25</v>
       </c>
       <c r="J74" t="n">
-        <v>5.150594216313028</v>
+        <v>5.082401069136825</v>
       </c>
       <c r="K74" t="n">
         <v>6.8</v>
       </c>
       <c r="L74" t="n">
-        <v>7.210935558633301</v>
+        <v>6.959238753871315</v>
       </c>
     </row>
     <row r="75">
@@ -3274,37 +3274,37 @@
         <v>7.4</v>
       </c>
       <c r="B75" t="n">
-        <v>7.155576668044792</v>
+        <v>7.68803279038677</v>
       </c>
       <c r="C75" t="n">
         <v>7.5</v>
       </c>
       <c r="D75" t="n">
-        <v>8.069241710619899</v>
+        <v>7.790671236747457</v>
       </c>
       <c r="E75" t="n">
         <v>5.75</v>
       </c>
       <c r="F75" t="n">
-        <v>6.371273479661621</v>
+        <v>5.967409513737732</v>
       </c>
       <c r="G75" t="n">
         <v>7.75</v>
       </c>
       <c r="H75" t="n">
-        <v>7.241035748821194</v>
+        <v>7.853390787398234</v>
       </c>
       <c r="I75" t="n">
         <v>6.25</v>
       </c>
       <c r="J75" t="n">
-        <v>5.025284987689906</v>
+        <v>5.083292361430489</v>
       </c>
       <c r="K75" t="n">
         <v>8.6</v>
       </c>
       <c r="L75" t="n">
-        <v>6.684866478556369</v>
+        <v>6.59563987083463</v>
       </c>
     </row>
     <row r="76">
@@ -3312,37 +3312,37 @@
         <v>8.6</v>
       </c>
       <c r="B76" t="n">
-        <v>7.746035054852745</v>
+        <v>8.227248278785252</v>
       </c>
       <c r="C76" t="n">
         <v>7.75</v>
       </c>
       <c r="D76" t="n">
-        <v>8.376723455262807</v>
+        <v>8.044801181111801</v>
       </c>
       <c r="E76" t="n">
         <v>9</v>
       </c>
       <c r="F76" t="n">
-        <v>7.569234664806386</v>
+        <v>7.580238309037052</v>
       </c>
       <c r="G76" t="n">
         <v>8.5</v>
       </c>
       <c r="H76" t="n">
-        <v>8.009704786574863</v>
+        <v>8.629381782026083</v>
       </c>
       <c r="I76" t="n">
         <v>7.25</v>
       </c>
       <c r="J76" t="n">
-        <v>6.899340910184455</v>
+        <v>6.679485279192743</v>
       </c>
       <c r="K76" t="n">
         <v>8.199999999999999</v>
       </c>
       <c r="L76" t="n">
-        <v>7.839952137780627</v>
+        <v>7.563813329810758</v>
       </c>
     </row>
     <row r="77">
@@ -3350,37 +3350,37 @@
         <v>7</v>
       </c>
       <c r="B77" t="n">
-        <v>6.163502545240049</v>
+        <v>6.753925087849621</v>
       </c>
       <c r="C77" t="n">
         <v>8.5</v>
       </c>
       <c r="D77" t="n">
-        <v>6.964994762805363</v>
+        <v>6.544055535080204</v>
       </c>
       <c r="E77" t="n">
         <v>6.5</v>
       </c>
       <c r="F77" t="n">
-        <v>5.626635484718371</v>
+        <v>5.214360511403664</v>
       </c>
       <c r="G77" t="n">
         <v>6.5</v>
       </c>
       <c r="H77" t="n">
-        <v>5.813594618709703</v>
+        <v>6.31372388552365</v>
       </c>
       <c r="I77" t="n">
         <v>5.5</v>
       </c>
       <c r="J77" t="n">
-        <v>4.172908316370024</v>
+        <v>4.234603049920191</v>
       </c>
       <c r="K77" t="n">
         <v>4.6</v>
       </c>
       <c r="L77" t="n">
-        <v>3.648986182414977</v>
+        <v>3.548119558810772</v>
       </c>
     </row>
     <row r="78">
@@ -3388,37 +3388,37 @@
         <v>7.8</v>
       </c>
       <c r="B78" t="n">
-        <v>7.359435532717272</v>
+        <v>7.86398583938042</v>
       </c>
       <c r="C78" t="n">
         <v>7.75</v>
       </c>
       <c r="D78" t="n">
-        <v>7.560275626091796</v>
+        <v>7.165706157287333</v>
       </c>
       <c r="E78" t="n">
         <v>7</v>
       </c>
       <c r="F78" t="n">
-        <v>7.271245060926598</v>
+        <v>7.240580551840806</v>
       </c>
       <c r="G78" t="n">
         <v>8.25</v>
       </c>
       <c r="H78" t="n">
-        <v>7.447447826093952</v>
+        <v>8.021087420508287</v>
       </c>
       <c r="I78" t="n">
         <v>6</v>
       </c>
       <c r="J78" t="n">
-        <v>6.201032366535554</v>
+        <v>6.085666383712512</v>
       </c>
       <c r="K78" t="n">
         <v>6.2</v>
       </c>
       <c r="L78" t="n">
-        <v>5.795666317817747</v>
+        <v>5.631385577653594</v>
       </c>
     </row>
     <row r="79">
@@ -3426,37 +3426,37 @@
         <v>8.6</v>
       </c>
       <c r="B79" t="n">
-        <v>8.193196749477657</v>
+        <v>8.72756365201051</v>
       </c>
       <c r="C79" t="n">
         <v>7.25</v>
       </c>
       <c r="D79" t="n">
-        <v>8.305326426084545</v>
+        <v>7.951423670334224</v>
       </c>
       <c r="E79" t="n">
         <v>7.75</v>
       </c>
       <c r="F79" t="n">
-        <v>7.615481910267145</v>
+        <v>7.591672653420287</v>
       </c>
       <c r="G79" t="n">
         <v>8.25</v>
       </c>
       <c r="H79" t="n">
-        <v>7.757469281726706</v>
+        <v>8.381911029619936</v>
       </c>
       <c r="I79" t="n">
         <v>5.75</v>
       </c>
       <c r="J79" t="n">
-        <v>7.258822474655961</v>
+        <v>7.151761508886956</v>
       </c>
       <c r="K79" t="n">
         <v>6.8</v>
       </c>
       <c r="L79" t="n">
-        <v>8.13237976581158</v>
+        <v>7.938154733402511</v>
       </c>
     </row>
     <row r="80">
@@ -3464,37 +3464,37 @@
         <v>5.6</v>
       </c>
       <c r="B80" t="n">
-        <v>6.656107766331822</v>
+        <v>7.237287999860349</v>
       </c>
       <c r="C80" t="n">
         <v>8</v>
       </c>
       <c r="D80" t="n">
-        <v>8.107359515841146</v>
+        <v>7.848388392612888</v>
       </c>
       <c r="E80" t="n">
         <v>4.5</v>
       </c>
       <c r="F80" t="n">
-        <v>5.736350841514397</v>
+        <v>5.217430995204788</v>
       </c>
       <c r="G80" t="n">
         <v>6</v>
       </c>
       <c r="H80" t="n">
-        <v>5.920698677502401</v>
+        <v>6.471583101437679</v>
       </c>
       <c r="I80" t="n">
         <v>7.25</v>
       </c>
       <c r="J80" t="n">
-        <v>6.277925433701243</v>
+        <v>6.586999396405387</v>
       </c>
       <c r="K80" t="n">
         <v>4.6</v>
       </c>
       <c r="L80" t="n">
-        <v>4.353425420917793</v>
+        <v>4.564847742164642</v>
       </c>
     </row>
     <row r="81">
@@ -3502,37 +3502,37 @@
         <v>6.6</v>
       </c>
       <c r="B81" t="n">
-        <v>7.434265010121876</v>
+        <v>7.971196466981844</v>
       </c>
       <c r="C81" t="n">
         <v>7.75</v>
       </c>
       <c r="D81" t="n">
-        <v>7.60864952976702</v>
+        <v>7.226223237942609</v>
       </c>
       <c r="E81" t="n">
         <v>5</v>
       </c>
       <c r="F81" t="n">
-        <v>6.606662996232198</v>
+        <v>6.318574575692237</v>
       </c>
       <c r="G81" t="n">
         <v>5.25</v>
       </c>
       <c r="H81" t="n">
-        <v>6.947422639319409</v>
+        <v>7.518440354331574</v>
       </c>
       <c r="I81" t="n">
         <v>5.5</v>
       </c>
       <c r="J81" t="n">
-        <v>5.341988867992191</v>
+        <v>5.298079881817045</v>
       </c>
       <c r="K81" t="n">
         <v>4.6</v>
       </c>
       <c r="L81" t="n">
-        <v>3.915607242457758</v>
+        <v>3.988800833980696</v>
       </c>
     </row>
     <row r="82">
@@ -3540,37 +3540,37 @@
         <v>7</v>
       </c>
       <c r="B82" t="n">
-        <v>6.988222553334973</v>
+        <v>7.509898432181141</v>
       </c>
       <c r="C82" t="n">
         <v>8.5</v>
       </c>
       <c r="D82" t="n">
-        <v>8.567285343763174</v>
+        <v>8.293675188709521</v>
       </c>
       <c r="E82" t="n">
         <v>6.5</v>
       </c>
       <c r="F82" t="n">
-        <v>6.058813235476618</v>
+        <v>5.80942448301446</v>
       </c>
       <c r="G82" t="n">
         <v>8</v>
       </c>
       <c r="H82" t="n">
-        <v>6.819507619846282</v>
+        <v>7.508649670865402</v>
       </c>
       <c r="I82" t="n">
         <v>6.75</v>
       </c>
       <c r="J82" t="n">
-        <v>5.926872195529596</v>
+        <v>5.767251210064055</v>
       </c>
       <c r="K82" t="n">
         <v>8.4</v>
       </c>
       <c r="L82" t="n">
-        <v>7.567479426159788</v>
+        <v>7.250288740429909</v>
       </c>
     </row>
     <row r="83">
@@ -3578,37 +3578,37 @@
         <v>6.8</v>
       </c>
       <c r="B83" t="n">
-        <v>6.132258246315369</v>
+        <v>6.657971826449275</v>
       </c>
       <c r="C83" t="n">
         <v>5.5</v>
       </c>
       <c r="D83" t="n">
-        <v>6.992174608174081</v>
+        <v>6.461867846936126</v>
       </c>
       <c r="E83" t="n">
         <v>4.5</v>
       </c>
       <c r="F83" t="n">
-        <v>4.807543068230762</v>
+        <v>3.967943067666714</v>
       </c>
       <c r="G83" t="n">
         <v>6</v>
       </c>
       <c r="H83" t="n">
-        <v>4.749377044903602</v>
+        <v>5.186038491771447</v>
       </c>
       <c r="I83" t="n">
         <v>5</v>
       </c>
       <c r="J83" t="n">
-        <v>5.416157385547618</v>
+        <v>5.46091140051597</v>
       </c>
       <c r="K83" t="n">
         <v>8.199999999999999</v>
       </c>
       <c r="L83" t="n">
-        <v>7.381010013401546</v>
+        <v>7.167861054169849</v>
       </c>
     </row>
     <row r="84">
@@ -3616,37 +3616,37 @@
         <v>7.6</v>
       </c>
       <c r="B84" t="n">
-        <v>7.969893216433849</v>
+        <v>8.440880442183285</v>
       </c>
       <c r="C84" t="n">
         <v>8</v>
       </c>
       <c r="D84" t="n">
-        <v>8.580251307527195</v>
+        <v>8.249834569737283</v>
       </c>
       <c r="E84" t="n">
         <v>8.75</v>
       </c>
       <c r="F84" t="n">
-        <v>7.924460708842727</v>
+        <v>8.022901475400797</v>
       </c>
       <c r="G84" t="n">
         <v>7.25</v>
       </c>
       <c r="H84" t="n">
-        <v>5.791715820010577</v>
+        <v>6.370185290673735</v>
       </c>
       <c r="I84" t="n">
         <v>6.5</v>
       </c>
       <c r="J84" t="n">
-        <v>6.41380000004152</v>
+        <v>6.263789886496258</v>
       </c>
       <c r="K84" t="n">
         <v>8.4</v>
       </c>
       <c r="L84" t="n">
-        <v>7.686480752810649</v>
+        <v>7.408487635527578</v>
       </c>
     </row>
     <row r="85">
@@ -3654,37 +3654,37 @@
         <v>7</v>
       </c>
       <c r="B85" t="n">
-        <v>6.220491246604353</v>
+        <v>6.773996408488352</v>
       </c>
       <c r="C85" t="n">
         <v>6</v>
       </c>
       <c r="D85" t="n">
-        <v>7.100421069656452</v>
+        <v>6.604605022814271</v>
       </c>
       <c r="E85" t="n">
         <v>5.5</v>
       </c>
       <c r="F85" t="n">
-        <v>5.587144456816622</v>
+        <v>5.124451345007676</v>
       </c>
       <c r="G85" t="n">
         <v>7.5</v>
       </c>
       <c r="H85" t="n">
-        <v>4.817767205543946</v>
+        <v>5.357242559155043</v>
       </c>
       <c r="I85" t="n">
         <v>3.75</v>
       </c>
       <c r="J85" t="n">
-        <v>4.477451664072041</v>
+        <v>4.506344981365505</v>
       </c>
       <c r="K85" t="n">
         <v>5</v>
       </c>
       <c r="L85" t="n">
-        <v>3.803288822696769</v>
+        <v>3.857805958818018</v>
       </c>
     </row>
     <row r="86">
@@ -3692,37 +3692,37 @@
         <v>8.4</v>
       </c>
       <c r="B86" t="n">
-        <v>7.724687455333944</v>
+        <v>8.249826157006954</v>
       </c>
       <c r="C86" t="n">
         <v>7.25</v>
       </c>
       <c r="D86" t="n">
-        <v>8.154366173379412</v>
+        <v>7.78386148441532</v>
       </c>
       <c r="E86" t="n">
         <v>8.25</v>
       </c>
       <c r="F86" t="n">
-        <v>7.39225949693911</v>
+        <v>7.42234403666574</v>
       </c>
       <c r="G86" t="n">
         <v>8.5</v>
       </c>
       <c r="H86" t="n">
-        <v>7.304109036247593</v>
+        <v>7.911536862233976</v>
       </c>
       <c r="I86" t="n">
         <v>7</v>
       </c>
       <c r="J86" t="n">
-        <v>6.784575717989264</v>
+        <v>6.612694605803071</v>
       </c>
       <c r="K86" t="n">
         <v>6.4</v>
       </c>
       <c r="L86" t="n">
-        <v>7.11879100454255</v>
+        <v>6.859408318484302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>